<commit_message>
Changed emotion calibration of BEAT memory file (used in BEAT scenario, FLEE-by-reversal-of-affect scenario and FLEE-by-reflected-feeling-evaluation scenario)
</commit_message>
<xml_diff>
--- a/ARSMemory/config/_v38/bw/pa.memory/ADAM_EC2_EAT/emotion_generation.xlsx
+++ b/ARSMemory/config/_v38/bw/pa.memory/ADAM_EC2_EAT/emotion_generation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>IMAGE</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>emotion name</t>
+  </si>
+  <si>
+    <t>EMOTION(A06_BEAT_BODO_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J32"/>
+      <selection activeCell="I2" sqref="I2:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,8 +550,8 @@
         <v>A06_BEAT_BODO_L01:ANGER</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("EMOTION(",H2,"){value=[",B2,"]; value_type=[BASICEMOTION]; emotionIntensity=[",C2,"]; sourceAggr=[",D2,"]; sourceLibid=[",E2,"]; sourcePleasure=[",F2,"]; sourceUnpleasure=[",G2,"]}")</f>
-        <v>EMOTION(A06_BEAT_BODO_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <f>CONCATENATE("EMOTION(",H2,"){value=[",B2,"]; value_type=[BASICEMOTION]; emotionIntensity=[",SUBSTITUTE(B2,",","."),"]; sourceAggr=[",SUBSTITUTE(D2,",","."),"]; sourceLibid=[",SUBSTITUTE(E2,",","."),"]; sourcePleasure=[",SUBSTITUTE(F2,",","."),"]; sourceUnpleasure=[",SUBSTITUTE(G2,",","."),"]}")</f>
+        <v>EMOTION(A06_BEAT_BODO_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE("ASSOCIATIONEMOTION(",H2,"){element=[\TPM:IMAGE:",A2,", \EMOTION:",H2,"]}")</f>
@@ -582,8 +585,8 @@
         <v>A06_BEAT_BODO_L01_I01:ANGER</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I32" si="1">CONCATENATE("EMOTION(",H3,"){value=[",B3,"]; value_type=[BASICEMOTION]; emotionIntensity=[",C3,"]; sourceAggr=[",D3,"]; sourceLibid=[",E3,"]; sourcePleasure=[",F3,"]; sourceUnpleasure=[",G3,"]}")</f>
-        <v>EMOTION(A06_BEAT_BODO_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <f t="shared" ref="I3:I32" si="1">CONCATENATE("EMOTION(",H3,"){value=[",B3,"]; value_type=[BASICEMOTION]; emotionIntensity=[",SUBSTITUTE(B3,",","."),"]; sourceAggr=[",SUBSTITUTE(D3,",","."),"]; sourceLibid=[",SUBSTITUTE(E3,",","."),"]; sourcePleasure=[",SUBSTITUTE(F3,",","."),"]; sourceUnpleasure=[",SUBSTITUTE(G3,",","."),"]}")</f>
+        <v>EMOTION(A06_BEAT_BODO_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J32" si="2">CONCATENATE("ASSOCIATIONEMOTION(",H3,"){element=[\TPM:IMAGE:",A3,", \EMOTION:",H3,"]}")</f>
@@ -618,7 +621,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A06_BEAT_BODO_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A06_BEAT_BODO_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="2"/>
@@ -653,7 +656,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A06_BEAT_BODO_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A06_BEAT_BODO_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="2"/>
@@ -688,7 +691,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
@@ -723,7 +726,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
@@ -758,7 +761,7 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
@@ -793,7 +796,7 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
@@ -828,7 +831,7 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
@@ -863,7 +866,7 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
@@ -898,7 +901,7 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I06:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I06:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
@@ -933,7 +936,7 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I07:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I07:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
@@ -968,7 +971,7 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I08:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I08:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
@@ -1003,7 +1006,7 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I09:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,3]; sourceAggr=[0,3]; sourceLibid=[0,4]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I09:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
@@ -1038,7 +1041,7 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="2"/>
@@ -1073,7 +1076,7 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="2"/>
@@ -1108,7 +1111,7 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="2"/>
@@ -1143,7 +1146,7 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="2"/>
@@ -1178,7 +1181,7 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="2"/>
@@ -1213,7 +1216,7 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="2"/>
@@ -1248,7 +1251,7 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="2"/>
@@ -1283,7 +1286,7 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0,1]; sourceAggr=[0,2]; sourceLibid=[0,15]; sourcePleasure=[0,05]; sourceUnpleasure=[0,25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="2"/>
@@ -1318,7 +1321,7 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="2"/>
@@ -1353,7 +1356,7 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="2"/>
@@ -1388,7 +1391,7 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="2"/>
@@ -1423,7 +1426,7 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="2"/>
@@ -1458,7 +1461,7 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="2"/>
@@ -1493,7 +1496,7 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0,6]; sourceAggr=[0,6]; sourceLibid=[0,2]; sourcePleasure=[0,1]; sourceUnpleasure=[0,6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="2"/>
@@ -1528,7 +1531,7 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A14_FLEE_BODO_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0,65]; sourceAggr=[0,11]; sourceLibid=[0,35]; sourcePleasure=[0,06]; sourceUnpleasure=[0,65]}</v>
+        <v>EMOTION(A14_FLEE_BODO_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.11]; sourceLibid=[0.35]; sourcePleasure=[0.06]; sourceUnpleasure=[0.65]}</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="2"/>
@@ -1563,7 +1566,7 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A14_FLEE_BODO_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0,65]; sourceAggr=[0,11]; sourceLibid=[0,35]; sourcePleasure=[0,06]; sourceUnpleasure=[0,65]}</v>
+        <v>EMOTION(A14_FLEE_BODO_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.11]; sourceLibid=[0.35]; sourcePleasure=[0.06]; sourceUnpleasure=[0.65]}</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="2"/>
@@ -1598,7 +1601,7 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A14_FLEE_BODO_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0,65]; sourceAggr=[0,11]; sourceLibid=[0,1]; sourcePleasure=[0,1]; sourceUnpleasure=[0,2]}</v>
+        <v>EMOTION(A14_FLEE_BODO_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.11]; sourceLibid=[0.1]; sourcePleasure=[0.1]; sourceUnpleasure=[0.2]}</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="2"/>
@@ -1607,6 +1610,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1617,7 +1621,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fixed bug in emotion generation excel sheet
</commit_message>
<xml_diff>
--- a/ARSMemory/config/_v38/bw/pa.memory/ADAM_EC2_EAT/emotion_generation.xlsx
+++ b/ARSMemory/config/_v38/bw/pa.memory/ADAM_EC2_EAT/emotion_generation.xlsx
@@ -480,7 +480,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I32"/>
+      <selection activeCell="J2" sqref="J2:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,8 +550,8 @@
         <v>A06_BEAT_BODO_L01:ANGER</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("EMOTION(",H2,"){value=[",B2,"]; value_type=[BASICEMOTION]; emotionIntensity=[",SUBSTITUTE(B2,",","."),"]; sourceAggr=[",SUBSTITUTE(D2,",","."),"]; sourceLibid=[",SUBSTITUTE(E2,",","."),"]; sourcePleasure=[",SUBSTITUTE(F2,",","."),"]; sourceUnpleasure=[",SUBSTITUTE(G2,",","."),"]}")</f>
-        <v>EMOTION(A06_BEAT_BODO_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <f>CONCATENATE("EMOTION(",H2,"){value=[",B2,"]; value_type=[BASICEMOTION]; emotionIntensity=[",SUBSTITUTE(C2,",","."),"]; sourceAggr=[",SUBSTITUTE(D2,",","."),"]; sourceLibid=[",SUBSTITUTE(E2,",","."),"]; sourcePleasure=[",SUBSTITUTE(F2,",","."),"]; sourceUnpleasure=[",SUBSTITUTE(G2,",","."),"]}")</f>
+        <v>EMOTION(A06_BEAT_BODO_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE("ASSOCIATIONEMOTION(",H2,"){element=[\TPM:IMAGE:",A2,", \EMOTION:",H2,"]}")</f>
@@ -585,8 +585,8 @@
         <v>A06_BEAT_BODO_L01_I01:ANGER</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I32" si="1">CONCATENATE("EMOTION(",H3,"){value=[",B3,"]; value_type=[BASICEMOTION]; emotionIntensity=[",SUBSTITUTE(B3,",","."),"]; sourceAggr=[",SUBSTITUTE(D3,",","."),"]; sourceLibid=[",SUBSTITUTE(E3,",","."),"]; sourcePleasure=[",SUBSTITUTE(F3,",","."),"]; sourceUnpleasure=[",SUBSTITUTE(G3,",","."),"]}")</f>
-        <v>EMOTION(A06_BEAT_BODO_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <f t="shared" ref="I3:I32" si="1">CONCATENATE("EMOTION(",H3,"){value=[",B3,"]; value_type=[BASICEMOTION]; emotionIntensity=[",SUBSTITUTE(C3,",","."),"]; sourceAggr=[",SUBSTITUTE(D3,",","."),"]; sourceLibid=[",SUBSTITUTE(E3,",","."),"]; sourcePleasure=[",SUBSTITUTE(F3,",","."),"]; sourceUnpleasure=[",SUBSTITUTE(G3,",","."),"]}")</f>
+        <v>EMOTION(A06_BEAT_BODO_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J32" si="2">CONCATENATE("ASSOCIATIONEMOTION(",H3,"){element=[\TPM:IMAGE:",A3,", \EMOTION:",H3,"]}")</f>
@@ -621,7 +621,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A06_BEAT_BODO_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A06_BEAT_BODO_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="2"/>
@@ -656,7 +656,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A06_BEAT_BODO_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A06_BEAT_BODO_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="2"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
@@ -726,7 +726,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
@@ -761,7 +761,7 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
@@ -796,7 +796,7 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
@@ -831,7 +831,7 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
@@ -866,7 +866,7 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I06:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I06:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
@@ -936,7 +936,7 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I07:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I07:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
@@ -971,7 +971,7 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I08:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I08:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A10_DIVIDE_CAKE_L01_I09:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A10_DIVIDE_CAKE_L01_I09:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.3]; sourceAggr=[0.3]; sourceLibid=[0.4]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="2"/>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="2"/>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="2"/>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="2"/>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="2"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="2"/>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[ANGER]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANGER){value=[ANGER]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="2"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
+        <v>EMOTION(A12_EAT_CAKE_L01_I03:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0.1]; sourceAggr=[0.2]; sourceLibid=[0.15]; sourcePleasure=[0.05]; sourceUnpleasure=[0.25]}</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="2"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="2"/>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I01:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="2"/>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I02:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="2"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I03:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="2"/>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I04:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="2"/>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A13_GIVE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[GUILT]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
+        <v>EMOTION(A13_GIVE_CAKE_L01_I05:GUILT){value=[GUILT]; value_type=[BASICEMOTION]; emotionIntensity=[0.6]; sourceAggr=[0.6]; sourceLibid=[0.2]; sourcePleasure=[0.1]; sourceUnpleasure=[0.6]}</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="2"/>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A14_FLEE_BODO_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.11]; sourceLibid=[0.35]; sourcePleasure=[0.06]; sourceUnpleasure=[0.65]}</v>
+        <v>EMOTION(A14_FLEE_BODO_L01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0.65]; sourceAggr=[0.11]; sourceLibid=[0.35]; sourcePleasure=[0.06]; sourceUnpleasure=[0.65]}</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="2"/>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A14_FLEE_BODO_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.11]; sourceLibid=[0.35]; sourcePleasure=[0.06]; sourceUnpleasure=[0.65]}</v>
+        <v>EMOTION(A14_FLEE_BODO_L01_I01:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0.65]; sourceAggr=[0.11]; sourceLibid=[0.35]; sourcePleasure=[0.06]; sourceUnpleasure=[0.65]}</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="2"/>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" si="1"/>
-        <v>EMOTION(A14_FLEE_BODO_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[ANXIETY]; sourceAggr=[0.11]; sourceLibid=[0.1]; sourcePleasure=[0.1]; sourceUnpleasure=[0.2]}</v>
+        <v>EMOTION(A14_FLEE_BODO_L01_I02:ANXIETY){value=[ANXIETY]; value_type=[BASICEMOTION]; emotionIntensity=[0.65]; sourceAggr=[0.11]; sourceLibid=[0.1]; sourcePleasure=[0.1]; sourceUnpleasure=[0.2]}</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="2"/>

</xml_diff>